<commit_message>
Working Fuzzy V LookUp
Achieved 85% accuracy over sample data set

TODO: Improve tokenization algorithm for typos

Added JupyterNotebook for quick result analysis
</commit_message>
<xml_diff>
--- a/Sample_Dataset/Primary_Reference_Table.xlsx
+++ b/Sample_Dataset/Primary_Reference_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luislascano01/Documents/Sabadell/Covenants_Matching/AI_VLookUp/Sample_Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{996B3027-2DCD-0F4F-8A8D-06C3FD134B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6342EB1C-D36A-5544-AB85-6A413A53FEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" xr2:uid="{AA52B1F4-6BB6-F249-9A3E-614D06AF30CA}"/>
+    <workbookView xWindow="17340" yWindow="940" windowWidth="17060" windowHeight="21260" xr2:uid="{AA52B1F4-6BB6-F249-9A3E-614D06AF30CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary_Reference_Table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="241">
   <si>
     <t>Address</t>
   </si>
@@ -731,6 +731,18 @@
   </si>
   <si>
     <t>Grupo Meximining</t>
+  </si>
+  <si>
+    <t>Flat Ridge 4 Wind, LLC</t>
+  </si>
+  <si>
+    <t>ONE SOUTH WACKER DRIVE SUITE 1800, Chicago, USA</t>
+  </si>
+  <si>
+    <t>Flat Ridges 5 Wind Energy, LLC</t>
+  </si>
+  <si>
+    <t>Renewable Energy</t>
   </si>
 </sst>
 </file>
@@ -1591,10 +1603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F689D17A-95C1-6D47-AC04-865FE7DB841E}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="183" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1602,6 +1614,7 @@
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3004,7 +3017,36 @@
         <v>232</v>
       </c>
     </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>237</v>
+      </c>
+      <c r="C101" t="s">
+        <v>238</v>
+      </c>
+      <c r="D101" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>239</v>
+      </c>
+      <c r="C102" t="s">
+        <v>238</v>
+      </c>
+      <c r="D102" t="s">
+        <v>240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Compare by ID + Similarity Coefficient
Completed the compare by ID functionality so it through the YAML one may se what the key columns for each side of the Bidirectional comparison.

Full priority is given for full matches over the key columns.

TODO: Fix penalization for not including information under certain columns. It has been analyzed that reference entries that have more columns filled are most likely to be matched in average with any random entry.
</commit_message>
<xml_diff>
--- a/Sample_Dataset/Primary_Reference_Table.xlsx
+++ b/Sample_Dataset/Primary_Reference_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luislascano01/Documents/Sabadell/Covenants_Matching/AI_VLookUp/Sample_Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6C94A4-1838-4849-8A20-A3FFA4924D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFCDE6A-DF3F-3645-A6B8-2C9471F8B3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="940" windowWidth="17060" windowHeight="21260" xr2:uid="{AA52B1F4-6BB6-F249-9A3E-614D06AF30CA}"/>
+    <workbookView xWindow="17340" yWindow="920" windowWidth="17060" windowHeight="21260" xr2:uid="{AA52B1F4-6BB6-F249-9A3E-614D06AF30CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary_Reference_Table" sheetId="1" r:id="rId1"/>
@@ -1605,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F689D17A-95C1-6D47-AC04-865FE7DB841E}">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Implemented top entries Sorting
Options:
    - Jaccard distance
    - Damerau distance
</commit_message>
<xml_diff>
--- a/Sample_Dataset/Primary_Reference_Table.xlsx
+++ b/Sample_Dataset/Primary_Reference_Table.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luislascano01/Documents/Sabadell/Covenants_Matching/AI_VLookUp/Sample_Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFCDE6A-DF3F-3645-A6B8-2C9471F8B3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26D979F-3373-B84F-B760-47960E344A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17340" yWindow="920" windowWidth="17060" windowHeight="21260" xr2:uid="{AA52B1F4-6BB6-F249-9A3E-614D06AF30CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary_Reference_Table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="246">
   <si>
     <t>Address</t>
   </si>
@@ -743,6 +756,21 @@
   </si>
   <si>
     <t>Renewable Energy</t>
+  </si>
+  <si>
+    <t>Banco Pichincha</t>
+  </si>
+  <si>
+    <t>Avenida Amazonas N35-211 y Japon, Quito, Ecuador</t>
+  </si>
+  <si>
+    <t>Av. Libertadores, Monterrey, Mexico</t>
+  </si>
+  <si>
+    <t>PetroEcuador</t>
+  </si>
+  <si>
+    <t>Alpallana E8-86 Y Av. , 6 de Diciembre, Quito, Ecuador</t>
   </si>
 </sst>
 </file>
@@ -1605,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F689D17A-95C1-6D47-AC04-865FE7DB841E}">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2896,10 +2924,10 @@
         <v>10091</v>
       </c>
       <c r="B92" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
       <c r="C92" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
       <c r="D92" t="s">
         <v>116</v>
@@ -2910,13 +2938,13 @@
         <v>10092</v>
       </c>
       <c r="B93" t="s">
-        <v>163</v>
+        <v>241</v>
       </c>
       <c r="C93" t="s">
-        <v>164</v>
+        <v>242</v>
       </c>
       <c r="D93" t="s">
-        <v>165</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2955,7 +2983,7 @@
         <v>236</v>
       </c>
       <c r="C96" t="s">
-        <v>175</v>
+        <v>243</v>
       </c>
       <c r="D96" t="s">
         <v>165</v>

</xml_diff>